<commit_message>
Add onPrem Cudf 25.10 Nvidia dataset.
</commit_message>
<xml_diff>
--- a/excel/Perf_Comparison_Ex_Nex_AWS_S3_SF100_huge_chunks.xlsx
+++ b/excel/Perf_Comparison_Ex_Nex_AWS_S3_SF100_huge_chunks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnb/git/perfleap/presto_benchmarking/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C5DE86-74DC-8445-87A6-3385F478AAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADFF576-F854-9A48-B2AB-5AD30CB4814C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="1160" windowWidth="46560" windowHeight="25940" activeTab="9" xr2:uid="{FB6AB903-1CF7-2A4F-A7F8-58E6A057D4B0}"/>
+    <workbookView xWindow="660" yWindow="1160" windowWidth="46560" windowHeight="25940" activeTab="8" xr2:uid="{FB6AB903-1CF7-2A4F-A7F8-58E6A057D4B0}"/>
   </bookViews>
   <sheets>
     <sheet name="nex_aws_nvidia_sf100" sheetId="29" r:id="rId1"/>
@@ -1276,11 +1276,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8002,13 +8001,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6D03CC30-BB5F-7E45-9CC1-57463CCC6749}" name="nex_hugechunk_nvidia_aws_cuda2510" displayName="nex_hugechunk_nvidia_aws_cuda2510" ref="A1:G22" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G22" xr:uid="{6D03CC30-BB5F-7E45-9CC1-57463CCC6749}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{74B61E47-749E-C44B-A526-B2E51FCF813D}" uniqueName="1" name="queryName" queryTableFieldId="1" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{9167CE70-4BD1-F940-8029-6354400915B7}" uniqueName="2" name="scaleFactor" queryTableFieldId="2" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{74B61E47-749E-C44B-A526-B2E51FCF813D}" uniqueName="1" name="queryName" queryTableFieldId="1" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{9167CE70-4BD1-F940-8029-6354400915B7}" uniqueName="2" name="scaleFactor" queryTableFieldId="2" dataDxfId="34"/>
     <tableColumn id="3" xr3:uid="{C3AFEED9-3E78-C74C-86FA-6B567DBE5445}" uniqueName="3" name="timeMillsecs" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{703B77F0-E8A1-6241-8B33-A3ED8C389947}" uniqueName="4" name="queryStats.createTime" queryTableFieldId="4" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{68AFCF23-6DF8-644F-8697-369F1309C475}" uniqueName="5" name="queryId" queryTableFieldId="5" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{964CB8F1-FA6F-E042-8FF2-8ECC2A271E9F}" uniqueName="6" name="queryStats.elapsedTime" queryTableFieldId="6" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{B567C47B-1AE6-7640-B166-418BA026C607}" uniqueName="7" name="state" queryTableFieldId="7" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{703B77F0-E8A1-6241-8B33-A3ED8C389947}" uniqueName="4" name="queryStats.createTime" queryTableFieldId="4" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{68AFCF23-6DF8-644F-8697-369F1309C475}" uniqueName="5" name="queryId" queryTableFieldId="5" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{964CB8F1-FA6F-E042-8FF2-8ECC2A271E9F}" uniqueName="6" name="queryStats.elapsedTime" queryTableFieldId="6" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{B567C47B-1AE6-7640-B166-418BA026C607}" uniqueName="7" name="state" queryTableFieldId="7" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8018,13 +8017,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B733BFFD-0EBE-CA4A-8F1D-0A55F9323507}" name="ex_hugechunk_nvidia_aws_cuda2510" displayName="ex_hugechunk_nvidia_aws_cuda2510" ref="A1:G22" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G22" xr:uid="{B733BFFD-0EBE-CA4A-8F1D-0A55F9323507}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AF58BEF8-1F29-2944-95EA-555CA855DCBB}" uniqueName="1" name="queryName" queryTableFieldId="1" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{37DCA903-EC26-3A4F-8CB1-91CC6E2FD480}" uniqueName="2" name="scaleFactor" queryTableFieldId="2" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{AF58BEF8-1F29-2944-95EA-555CA855DCBB}" uniqueName="1" name="queryName" queryTableFieldId="1" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{37DCA903-EC26-3A4F-8CB1-91CC6E2FD480}" uniqueName="2" name="scaleFactor" queryTableFieldId="2" dataDxfId="28"/>
     <tableColumn id="3" xr3:uid="{ABA9F32E-CADF-1A49-A6BC-D816F710F0F3}" uniqueName="3" name="timeMillsecs" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{A2148592-9BF9-F941-A6D7-5213C0C0B7C5}" uniqueName="4" name="queryStats.createTime" queryTableFieldId="4" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{0AEFA9AF-239F-9642-A0EA-E957EB440BD1}" uniqueName="5" name="queryId" queryTableFieldId="5" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{4AB5475B-E5DD-9849-9596-D5262EDC9C87}" uniqueName="6" name="queryStats.elapsedTime" queryTableFieldId="6" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{D3CA01F1-4A26-AD4F-859A-EFCDDAD7BC17}" uniqueName="7" name="state" queryTableFieldId="7" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{A2148592-9BF9-F941-A6D7-5213C0C0B7C5}" uniqueName="4" name="queryStats.createTime" queryTableFieldId="4" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{0AEFA9AF-239F-9642-A0EA-E957EB440BD1}" uniqueName="5" name="queryId" queryTableFieldId="5" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{4AB5475B-E5DD-9849-9596-D5262EDC9C87}" uniqueName="6" name="queryStats.elapsedTime" queryTableFieldId="6" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{D3CA01F1-4A26-AD4F-859A-EFCDDAD7BC17}" uniqueName="7" name="state" queryTableFieldId="7" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8034,13 +8033,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D484EAF3-0597-AA4D-9ACF-5586F06E1F8C}" name="ex_nvidia_aws_cuda2510" displayName="ex_nvidia_aws_cuda2510" ref="A1:G22" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G22" xr:uid="{D484EAF3-0597-AA4D-9ACF-5586F06E1F8C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{10D3AE95-8AAE-1340-8614-D38E7B628FC7}" uniqueName="1" name="queryName" queryTableFieldId="1" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{5577293E-AA85-F24D-85DC-1237F4698408}" uniqueName="2" name="scaleFactor" queryTableFieldId="2" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{10D3AE95-8AAE-1340-8614-D38E7B628FC7}" uniqueName="1" name="queryName" queryTableFieldId="1" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{5577293E-AA85-F24D-85DC-1237F4698408}" uniqueName="2" name="scaleFactor" queryTableFieldId="2" dataDxfId="22"/>
     <tableColumn id="3" xr3:uid="{574A855A-C1AF-694A-BCF1-BA3C605C953A}" uniqueName="3" name="timeMillsecs" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{B154D74E-2CF6-6F4D-8C30-F741EC08AFB5}" uniqueName="4" name="queryStats.createTime" queryTableFieldId="4" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{A4048C76-5A69-5345-AF46-FD49185DFBAF}" uniqueName="5" name="queryId" queryTableFieldId="5" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{667D7E2D-1A95-AD47-85A0-A2C1D5C44929}" uniqueName="6" name="queryStats.elapsedTime" queryTableFieldId="6" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{99BE4170-A556-FA47-B404-EE8B2F9364C1}" uniqueName="7" name="state" queryTableFieldId="7" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{B154D74E-2CF6-6F4D-8C30-F741EC08AFB5}" uniqueName="4" name="queryStats.createTime" queryTableFieldId="4" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{A4048C76-5A69-5345-AF46-FD49185DFBAF}" uniqueName="5" name="queryId" queryTableFieldId="5" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{667D7E2D-1A95-AD47-85A0-A2C1D5C44929}" uniqueName="6" name="queryStats.elapsedTime" queryTableFieldId="6" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{99BE4170-A556-FA47-B404-EE8B2F9364C1}" uniqueName="7" name="state" queryTableFieldId="7" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8050,13 +8049,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BB86219A-6F94-CF42-AE95-6284EDA11A99}" name="nex_nvidia_aws_cuda2510" displayName="nex_nvidia_aws_cuda2510" ref="A1:G24" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G24" xr:uid="{BB86219A-6F94-CF42-AE95-6284EDA11A99}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{03B42792-11CE-6F47-864A-DACC0DADBD4C}" uniqueName="1" name="queryName" queryTableFieldId="1" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{F2BCC1C0-C490-6444-8A06-DF771A594139}" uniqueName="2" name="scaleFactor" queryTableFieldId="2" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{03B42792-11CE-6F47-864A-DACC0DADBD4C}" uniqueName="1" name="queryName" queryTableFieldId="1" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{F2BCC1C0-C490-6444-8A06-DF771A594139}" uniqueName="2" name="scaleFactor" queryTableFieldId="2" dataDxfId="16"/>
     <tableColumn id="3" xr3:uid="{9720C8ED-C1B4-AB47-B7B7-C0B039709DE6}" uniqueName="3" name="timeMillsecs" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{7F039CFB-65B8-D349-8C1C-14E2192D14D5}" uniqueName="4" name="queryStats.createTime" queryTableFieldId="4" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{F7B73966-2565-5F4E-8A1C-F75C10AAB7AE}" uniqueName="5" name="queryId" queryTableFieldId="5" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{ED9E9911-AEB2-D244-9863-D51000BDC481}" uniqueName="6" name="queryStats.elapsedTime" queryTableFieldId="6" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{4C496B99-F979-EE4A-A55E-49A28A710AF9}" uniqueName="7" name="state" queryTableFieldId="7" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{7F039CFB-65B8-D349-8C1C-14E2192D14D5}" uniqueName="4" name="queryStats.createTime" queryTableFieldId="4" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{F7B73966-2565-5F4E-8A1C-F75C10AAB7AE}" uniqueName="5" name="queryId" queryTableFieldId="5" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{ED9E9911-AEB2-D244-9863-D51000BDC481}" uniqueName="6" name="queryStats.elapsedTime" queryTableFieldId="6" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{4C496B99-F979-EE4A-A55E-49A28A710AF9}" uniqueName="7" name="state" queryTableFieldId="7" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9012,7 +9011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{598218FA-D521-4840-8389-532D3A7ECCF2}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB30" sqref="AB30"/>
     </sheetView>
   </sheetViews>
@@ -9689,10 +9688,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>26</v>
       </c>
       <c r="C2">
@@ -9701,13 +9700,13 @@
       <c r="D2" s="1">
         <v>45924.578301793983</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s">
         <v>155</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" t="s">
         <v>156</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="2">
@@ -9715,10 +9714,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>26</v>
       </c>
       <c r="C3">
@@ -9727,13 +9726,13 @@
       <c r="D3" s="1">
         <v>45924.578388981485</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" t="s">
         <v>158</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" t="s">
         <v>4</v>
       </c>
       <c r="I3" s="2">
@@ -9741,10 +9740,10 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>26</v>
       </c>
       <c r="C4">
@@ -9753,13 +9752,13 @@
       <c r="D4" s="1">
         <v>45924.578569606485</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>159</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>160</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>4</v>
       </c>
       <c r="I4" s="2">
@@ -9767,10 +9766,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>26</v>
       </c>
       <c r="C5">
@@ -9779,13 +9778,13 @@
       <c r="D5" s="1">
         <v>45924.578707731482</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" t="s">
         <v>161</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" t="s">
         <v>162</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="2">
@@ -9793,10 +9792,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>26</v>
       </c>
       <c r="C6">
@@ -9805,13 +9804,13 @@
       <c r="D6" s="1">
         <v>45924.578787326391</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" t="s">
         <v>163</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" t="s">
         <v>164</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" t="s">
         <v>4</v>
       </c>
       <c r="I6" s="2">
@@ -9819,10 +9818,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>26</v>
       </c>
       <c r="C7">
@@ -9831,13 +9830,13 @@
       <c r="D7" s="1">
         <v>45924.579008622684</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" t="s">
         <v>165</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" t="s">
         <v>166</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" t="s">
         <v>4</v>
       </c>
       <c r="I7" s="2">
@@ -9845,10 +9844,10 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>26</v>
       </c>
       <c r="C8">
@@ -9857,13 +9856,13 @@
       <c r="D8" s="1">
         <v>45924.579079432871</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" t="s">
         <v>167</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" t="s">
         <v>168</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" t="s">
         <v>4</v>
       </c>
       <c r="I8" s="2">
@@ -9871,10 +9870,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>26</v>
       </c>
       <c r="C9">
@@ -9883,13 +9882,13 @@
       <c r="D9" s="1">
         <v>45924.579278020836</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" t="s">
         <v>169</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" t="s">
         <v>170</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" t="s">
         <v>4</v>
       </c>
       <c r="I9" s="2">
@@ -9897,10 +9896,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>26</v>
       </c>
       <c r="C10">
@@ -9909,13 +9908,13 @@
       <c r="D10" s="1">
         <v>45924.579715763888</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" t="s">
         <v>171</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" t="s">
         <v>172</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" t="s">
         <v>4</v>
       </c>
       <c r="I10" s="2">
@@ -9923,10 +9922,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>26</v>
       </c>
       <c r="C11">
@@ -9935,13 +9934,13 @@
       <c r="D11" s="1">
         <v>45924.580273506945</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" t="s">
         <v>173</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" t="s">
         <v>174</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" t="s">
         <v>4</v>
       </c>
       <c r="I11" s="2">
@@ -9949,10 +9948,10 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>26</v>
       </c>
       <c r="C12">
@@ -9961,13 +9960,13 @@
       <c r="D12" s="1">
         <v>45924.580588611112</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" t="s">
         <v>176</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" t="s">
         <v>177</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" t="s">
         <v>4</v>
       </c>
       <c r="I12" s="2">
@@ -9975,10 +9974,10 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>26</v>
       </c>
       <c r="C13">
@@ -9987,13 +9986,13 @@
       <c r="D13" s="1">
         <v>45924.580762835649</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" t="s">
         <v>178</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" t="s">
         <v>179</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" t="s">
         <v>4</v>
       </c>
       <c r="I13" s="2">
@@ -10001,10 +10000,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
       <c r="C14">
@@ -10013,13 +10012,13 @@
       <c r="D14" s="1">
         <v>45924.580930428237</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" t="s">
         <v>180</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" t="s">
         <v>181</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" t="s">
         <v>4</v>
       </c>
       <c r="I14" s="2">
@@ -10027,10 +10026,10 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" t="s">
         <v>26</v>
       </c>
       <c r="C15">
@@ -10039,13 +10038,13 @@
       <c r="D15" s="1">
         <v>45924.581021458333</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" t="s">
         <v>182</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" t="s">
         <v>183</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" t="s">
         <v>4</v>
       </c>
       <c r="I15" s="2">
@@ -10053,10 +10052,10 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" t="s">
         <v>26</v>
       </c>
       <c r="C16">
@@ -10065,13 +10064,13 @@
       <c r="D16" s="1">
         <v>45924.581239120373</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" t="s">
         <v>184</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" t="s">
         <v>185</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" t="s">
         <v>4</v>
       </c>
       <c r="I16" s="2">
@@ -10079,10 +10078,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" t="s">
         <v>26</v>
       </c>
       <c r="C17">
@@ -10091,13 +10090,13 @@
       <c r="D17" s="1">
         <v>45924.581401620373</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" t="s">
         <v>186</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" t="s">
         <v>187</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" t="s">
         <v>4</v>
       </c>
       <c r="I17" s="2">
@@ -10105,10 +10104,10 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" t="s">
         <v>26</v>
       </c>
       <c r="C18">
@@ -10117,13 +10116,13 @@
       <c r="D18" s="1">
         <v>45924.581569849535</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" t="s">
         <v>188</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" t="s">
         <v>189</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" t="s">
         <v>4</v>
       </c>
       <c r="I18" s="2">
@@ -10131,10 +10130,10 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" t="s">
         <v>26</v>
       </c>
       <c r="C19">
@@ -10143,13 +10142,13 @@
       <c r="D19" s="1">
         <v>45924.581819884261</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" t="s">
         <v>190</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" t="s">
         <v>191</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" t="s">
         <v>4</v>
       </c>
       <c r="I19" s="2">
@@ -10157,10 +10156,10 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>26</v>
       </c>
       <c r="C20">
@@ -10169,13 +10168,13 @@
       <c r="D20" s="1">
         <v>45924.581920023149</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" t="s">
         <v>192</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" t="s">
         <v>193</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" t="s">
         <v>4</v>
       </c>
       <c r="I20" s="2">
@@ -10183,10 +10182,10 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" t="s">
         <v>26</v>
       </c>
       <c r="C21">
@@ -10195,13 +10194,13 @@
       <c r="D21" s="1">
         <v>45924.582019930553</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" t="s">
         <v>194</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" t="s">
         <v>195</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" t="s">
         <v>4</v>
       </c>
       <c r="I21" s="2">
@@ -10209,10 +10208,10 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="C22">
@@ -10221,13 +10220,13 @@
       <c r="D22" s="1">
         <v>45924.58263571759</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" t="s">
         <v>196</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" t="s">
         <v>197</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" t="s">
         <v>4</v>
       </c>
       <c r="I22" s="2">
@@ -10288,10 +10287,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>26</v>
       </c>
       <c r="C2">
@@ -10300,13 +10299,13 @@
       <c r="D2" s="1">
         <v>45924.573159594911</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s">
         <v>115</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" t="s">
         <v>116</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="2">
@@ -10315,10 +10314,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>26</v>
       </c>
       <c r="C3">
@@ -10327,13 +10326,13 @@
       <c r="D3" s="1">
         <v>45924.573244224535</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" t="s">
         <v>117</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" t="s">
         <v>118</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" t="s">
         <v>4</v>
       </c>
       <c r="I3" s="2">
@@ -10342,10 +10341,10 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>26</v>
       </c>
       <c r="C4">
@@ -10354,13 +10353,13 @@
       <c r="D4" s="1">
         <v>45924.57333053241</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>119</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>120</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>4</v>
       </c>
       <c r="I4" s="2">
@@ -10369,10 +10368,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>26</v>
       </c>
       <c r="C5">
@@ -10381,13 +10380,13 @@
       <c r="D5" s="1">
         <v>45924.573422511574</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" t="s">
         <v>121</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" t="s">
         <v>122</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="2">
@@ -10396,10 +10395,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>26</v>
       </c>
       <c r="C6">
@@ -10408,13 +10407,13 @@
       <c r="D6" s="1">
         <v>45924.573494965276</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" t="s">
         <v>123</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" t="s">
         <v>124</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" t="s">
         <v>4</v>
       </c>
       <c r="I6" s="2">
@@ -10423,10 +10422,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>26</v>
       </c>
       <c r="C7">
@@ -10435,13 +10434,13 @@
       <c r="D7" s="1">
         <v>45924.573584409722</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" t="s">
         <v>125</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" t="s">
         <v>126</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" t="s">
         <v>4</v>
       </c>
       <c r="I7" s="2">
@@ -10450,10 +10449,10 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>26</v>
       </c>
       <c r="C8">
@@ -10462,13 +10461,13 @@
       <c r="D8" s="1">
         <v>45924.573649965278</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" t="s">
         <v>127</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" t="s">
         <v>128</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" t="s">
         <v>4</v>
       </c>
       <c r="I8" s="2">
@@ -10477,10 +10476,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>26</v>
       </c>
       <c r="C9">
@@ -10489,13 +10488,13 @@
       <c r="D9" s="1">
         <v>45924.57374605324</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" t="s">
         <v>129</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" t="s">
         <v>130</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" t="s">
         <v>4</v>
       </c>
       <c r="I9" s="2">
@@ -10504,10 +10503,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>26</v>
       </c>
       <c r="C10">
@@ -10516,13 +10515,13 @@
       <c r="D10" s="1">
         <v>45924.573846354164</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" t="s">
         <v>131</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" t="s">
         <v>132</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" t="s">
         <v>4</v>
       </c>
       <c r="I10" s="2">
@@ -10531,10 +10530,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>26</v>
       </c>
       <c r="C11">
@@ -10543,13 +10542,13 @@
       <c r="D11" s="1">
         <v>45924.573951979168</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" t="s">
         <v>133</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" t="s">
         <v>134</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" t="s">
         <v>4</v>
       </c>
       <c r="I11" s="2">
@@ -10558,10 +10557,10 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>26</v>
       </c>
       <c r="C12">
@@ -10570,13 +10569,13 @@
       <c r="D12" s="1">
         <v>45924.57411533565</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" t="s">
         <v>136</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" t="s">
         <v>137</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" t="s">
         <v>4</v>
       </c>
       <c r="I12" s="2">
@@ -10585,10 +10584,10 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>26</v>
       </c>
       <c r="C13">
@@ -10597,13 +10596,13 @@
       <c r="D13" s="1">
         <v>45924.574192604166</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" t="s">
         <v>138</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" t="s">
         <v>139</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" t="s">
         <v>4</v>
       </c>
       <c r="I13" s="2">
@@ -10612,10 +10611,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
       <c r="C14">
@@ -10624,13 +10623,13 @@
       <c r="D14" s="1">
         <v>45924.574286261573</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" t="s">
         <v>140</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" t="s">
         <v>141</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" t="s">
         <v>4</v>
       </c>
       <c r="I14" s="2">
@@ -10639,10 +10638,10 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" t="s">
         <v>26</v>
       </c>
       <c r="C15">
@@ -10651,13 +10650,13 @@
       <c r="D15" s="1">
         <v>45924.574356168981</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" t="s">
         <v>142</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" t="s">
         <v>116</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" t="s">
         <v>4</v>
       </c>
       <c r="I15" s="2">
@@ -10666,10 +10665,10 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" t="s">
         <v>26</v>
       </c>
       <c r="C16">
@@ -10678,13 +10677,13 @@
       <c r="D16" s="1">
         <v>45924.574440937497</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" t="s">
         <v>143</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" t="s">
         <v>144</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" t="s">
         <v>4</v>
       </c>
       <c r="I16" s="2">
@@ -10693,10 +10692,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" t="s">
         <v>26</v>
       </c>
       <c r="C17">
@@ -10705,13 +10704,13 @@
       <c r="D17" s="1">
         <v>45924.574541689813</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" t="s">
         <v>145</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" t="s">
         <v>146</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" t="s">
         <v>4</v>
       </c>
       <c r="I17" s="2">
@@ -10720,10 +10719,10 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" t="s">
         <v>26</v>
       </c>
       <c r="C18">
@@ -10732,13 +10731,13 @@
       <c r="D18" s="1">
         <v>45924.574621527776</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" t="s">
         <v>147</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" t="s">
         <v>116</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" t="s">
         <v>4</v>
       </c>
       <c r="I18" s="2">
@@ -10747,10 +10746,10 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" t="s">
         <v>26</v>
       </c>
       <c r="C19">
@@ -10759,13 +10758,13 @@
       <c r="D19" s="1">
         <v>45924.574706736108</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" t="s">
         <v>148</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" t="s">
         <v>149</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" t="s">
         <v>4</v>
       </c>
       <c r="I19" s="2">
@@ -10774,10 +10773,10 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>26</v>
       </c>
       <c r="C20">
@@ -10786,13 +10785,13 @@
       <c r="D20" s="1">
         <v>45924.57477871528</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" t="s">
         <v>150</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" t="s">
         <v>151</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" t="s">
         <v>4</v>
       </c>
       <c r="I20" s="2">
@@ -10801,10 +10800,10 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" t="s">
         <v>26</v>
       </c>
       <c r="C21">
@@ -10813,13 +10812,13 @@
       <c r="D21" s="1">
         <v>45924.574858136577</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" t="s">
         <v>152</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" t="s">
         <v>74</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" t="s">
         <v>4</v>
       </c>
       <c r="I21" s="2">
@@ -10828,10 +10827,10 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="C22">
@@ -10840,13 +10839,13 @@
       <c r="D22" s="1">
         <v>45924.574961759259</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" t="s">
         <v>153</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" t="s">
         <v>154</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" t="s">
         <v>4</v>
       </c>
       <c r="I22" s="2">
@@ -10911,10 +10910,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>26</v>
       </c>
       <c r="C2">
@@ -10923,21 +10922,21 @@
       <c r="D2" s="1">
         <v>45924.450841493053</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s">
         <v>243</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>26</v>
       </c>
       <c r="C3">
@@ -10946,21 +10945,21 @@
       <c r="D3" s="1">
         <v>45924.450936782407</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" t="s">
         <v>244</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>26</v>
       </c>
       <c r="C4">
@@ -10969,21 +10968,21 @@
       <c r="D4" s="1">
         <v>45924.45102576389</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>245</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>246</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>26</v>
       </c>
       <c r="C5">
@@ -10992,21 +10991,21 @@
       <c r="D5" s="1">
         <v>45924.451126886575</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" t="s">
         <v>247</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" t="s">
         <v>248</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>26</v>
       </c>
       <c r="C6">
@@ -11015,21 +11014,21 @@
       <c r="D6" s="1">
         <v>45924.451213472224</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" t="s">
         <v>249</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" t="s">
         <v>250</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>26</v>
       </c>
       <c r="C7">
@@ -11038,21 +11037,21 @@
       <c r="D7" s="1">
         <v>45924.451313310186</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" t="s">
         <v>251</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" t="s">
         <v>252</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>26</v>
       </c>
       <c r="C8">
@@ -11061,21 +11060,21 @@
       <c r="D8" s="1">
         <v>45924.451379849539</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" t="s">
         <v>253</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" t="s">
         <v>254</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>26</v>
       </c>
       <c r="C9">
@@ -11084,21 +11083,21 @@
       <c r="D9" s="1">
         <v>45924.451461157405</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" t="s">
         <v>255</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" t="s">
         <v>256</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>26</v>
       </c>
       <c r="C10">
@@ -11107,21 +11106,21 @@
       <c r="D10" s="1">
         <v>45924.45156976852</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" t="s">
         <v>257</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" t="s">
         <v>258</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>26</v>
       </c>
       <c r="C11">
@@ -11130,21 +11129,21 @@
       <c r="D11" s="1">
         <v>45924.451688622685</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" t="s">
         <v>259</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" t="s">
         <v>260</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>26</v>
       </c>
       <c r="C12">
@@ -11153,21 +11152,21 @@
       <c r="D12" s="1">
         <v>45924.45217355324</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" t="s">
         <v>263</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" t="s">
         <v>264</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>26</v>
       </c>
       <c r="C13">
@@ -11176,21 +11175,21 @@
       <c r="D13" s="1">
         <v>45924.45225638889</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" t="s">
         <v>265</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" t="s">
         <v>266</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
       <c r="C14">
@@ -11199,21 +11198,21 @@
       <c r="D14" s="1">
         <v>45924.452359305556</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" t="s">
         <v>267</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" t="s">
         <v>268</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" t="s">
         <v>26</v>
       </c>
       <c r="C15">
@@ -11222,21 +11221,21 @@
       <c r="D15" s="1">
         <v>45924.452430486112</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" t="s">
         <v>269</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" t="s">
         <v>270</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" t="s">
         <v>26</v>
       </c>
       <c r="C16">
@@ -11245,21 +11244,21 @@
       <c r="D16" s="1">
         <v>45924.452523506945</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" t="s">
         <v>271</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" t="s">
         <v>272</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" t="s">
         <v>26</v>
       </c>
       <c r="C17">
@@ -11268,21 +11267,21 @@
       <c r="D17" s="1">
         <v>45924.452621412034</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" t="s">
         <v>273</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" t="s">
         <v>274</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" t="s">
         <v>26</v>
       </c>
       <c r="C18">
@@ -11291,21 +11290,21 @@
       <c r="D18" s="1">
         <v>45924.452702013892</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" t="s">
         <v>275</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" t="s">
         <v>276</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" t="s">
         <v>26</v>
       </c>
       <c r="C19">
@@ -11314,21 +11313,21 @@
       <c r="D19" s="1">
         <v>45924.452794108794</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" t="s">
         <v>277</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" t="s">
         <v>278</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>26</v>
       </c>
       <c r="C20">
@@ -11337,21 +11336,21 @@
       <c r="D20" s="1">
         <v>45924.452868333334</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" t="s">
         <v>279</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" t="s">
         <v>280</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" t="s">
         <v>26</v>
       </c>
       <c r="C21">
@@ -11360,21 +11359,21 @@
       <c r="D21" s="1">
         <v>45924.452948796294</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" t="s">
         <v>281</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" t="s">
         <v>282</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="C22">
@@ -11383,21 +11382,21 @@
       <c r="D22" s="1">
         <v>45924.453063657405</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" t="s">
         <v>283</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" t="s">
         <v>284</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" t="s">
         <v>135</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" t="s">
         <v>26</v>
       </c>
       <c r="C23">
@@ -11406,13 +11405,13 @@
       <c r="D23" s="1">
         <v>45924.45178333333</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" t="s">
         <v>261</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" t="s">
         <v>262</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -11465,10 +11464,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>26</v>
       </c>
       <c r="C2">
@@ -11477,21 +11476,21 @@
       <c r="D2" s="1">
         <v>45924.463562777775</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s">
         <v>198</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" t="s">
         <v>199</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>26</v>
       </c>
       <c r="C3">
@@ -11500,21 +11499,21 @@
       <c r="D3" s="1">
         <v>45924.463669548612</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" t="s">
         <v>200</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" t="s">
         <v>201</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>26</v>
       </c>
       <c r="C4">
@@ -11523,21 +11522,21 @@
       <c r="D4" s="1">
         <v>45924.463861805554</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>202</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>203</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>26</v>
       </c>
       <c r="C5">
@@ -11546,21 +11545,21 @@
       <c r="D5" s="1">
         <v>45924.464019050924</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" t="s">
         <v>204</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" t="s">
         <v>205</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>26</v>
       </c>
       <c r="C6">
@@ -11569,21 +11568,21 @@
       <c r="D6" s="1">
         <v>45924.464115821756</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" t="s">
         <v>206</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" t="s">
         <v>207</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>26</v>
       </c>
       <c r="C7">
@@ -11592,21 +11591,21 @@
       <c r="D7" s="1">
         <v>45924.464436875001</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" t="s">
         <v>208</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" t="s">
         <v>209</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>26</v>
       </c>
       <c r="C8">
@@ -11615,21 +11614,21 @@
       <c r="D8" s="1">
         <v>45924.4645155787</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" t="s">
         <v>210</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" t="s">
         <v>211</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>26</v>
       </c>
       <c r="C9">
@@ -11638,21 +11637,21 @@
       <c r="D9" s="1">
         <v>45924.464683078702</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" t="s">
         <v>212</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" t="s">
         <v>213</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>26</v>
       </c>
       <c r="C10">
@@ -11661,21 +11660,21 @@
       <c r="D10" s="1">
         <v>45924.465152118057</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" t="s">
         <v>214</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" t="s">
         <v>215</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>26</v>
       </c>
       <c r="C11">
@@ -11684,21 +11683,21 @@
       <c r="D11" s="1">
         <v>45924.465646828707</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" t="s">
         <v>216</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" t="s">
         <v>217</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" t="s">
         <v>135</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>26</v>
       </c>
       <c r="C12">
@@ -11707,21 +11706,21 @@
       <c r="D12" s="1">
         <v>45924.465866053244</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" t="s">
         <v>218</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" t="s">
         <v>219</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>26</v>
       </c>
       <c r="C13">
@@ -11730,21 +11729,21 @@
       <c r="D13" s="1">
         <v>45924.465947256947</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" t="s">
         <v>220</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" t="s">
         <v>221</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
       <c r="C14">
@@ -11753,21 +11752,21 @@
       <c r="D14" s="1">
         <v>45924.466131597219</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" t="s">
         <v>222</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" t="s">
         <v>223</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" t="s">
         <v>26</v>
       </c>
       <c r="C15">
@@ -11776,21 +11775,21 @@
       <c r="D15" s="1">
         <v>45924.466315532409</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" t="s">
         <v>224</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" t="s">
         <v>225</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" t="s">
         <v>26</v>
       </c>
       <c r="C16">
@@ -11799,21 +11798,21 @@
       <c r="D16" s="1">
         <v>45924.466406284722</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" t="s">
         <v>226</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" t="s">
         <v>227</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" t="s">
         <v>26</v>
       </c>
       <c r="C17">
@@ -11822,21 +11821,21 @@
       <c r="D17" s="1">
         <v>45924.466617824073</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" t="s">
         <v>228</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" t="s">
         <v>229</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" t="s">
         <v>26</v>
       </c>
       <c r="C18">
@@ -11845,21 +11844,21 @@
       <c r="D18" s="1">
         <v>45924.466777048612</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" t="s">
         <v>230</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" t="s">
         <v>231</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" t="s">
         <v>26</v>
       </c>
       <c r="C19">
@@ -11868,21 +11867,21 @@
       <c r="D19" s="1">
         <v>45924.466948946756</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" t="s">
         <v>232</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" t="s">
         <v>233</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>26</v>
       </c>
       <c r="C20">
@@ -11891,21 +11890,21 @@
       <c r="D20" s="1">
         <v>45924.467263611114</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" t="s">
         <v>234</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" t="s">
         <v>235</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" t="s">
         <v>26</v>
       </c>
       <c r="C21">
@@ -11914,21 +11913,21 @@
       <c r="D21" s="1">
         <v>45924.467366597222</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" t="s">
         <v>236</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" t="s">
         <v>128</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="C22">
@@ -11937,21 +11936,21 @@
       <c r="D22" s="1">
         <v>45924.467471516204</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" t="s">
         <v>237</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" t="s">
         <v>238</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" t="s">
         <v>26</v>
       </c>
       <c r="C23">
@@ -11960,21 +11959,21 @@
       <c r="D23" s="1">
         <v>45924.46805369213</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" t="s">
         <v>239</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" t="s">
         <v>240</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="A24" t="s">
         <v>135</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" t="s">
         <v>26</v>
       </c>
       <c r="C24">
@@ -11983,13 +11982,13 @@
       <c r="D24" s="1">
         <v>45924.470070648145</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" t="s">
         <v>241</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" t="s">
         <v>242</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" t="s">
         <v>175</v>
       </c>
     </row>
@@ -12021,7 +12020,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12059,10 +12058,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>26</v>
       </c>
       <c r="C2">
@@ -12071,21 +12070,21 @@
       <c r="D2" s="1">
         <v>45924.615297118056</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s">
         <v>285</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" t="s">
         <v>286</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>26</v>
       </c>
       <c r="C3">
@@ -12094,21 +12093,21 @@
       <c r="D3" s="1">
         <v>45924.615363831021</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" t="s">
         <v>287</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" t="s">
         <v>166</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>26</v>
       </c>
       <c r="C4">
@@ -12117,21 +12116,21 @@
       <c r="D4" s="1">
         <v>45924.615426539349</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>288</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>289</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>26</v>
       </c>
       <c r="C5">
@@ -12140,21 +12139,21 @@
       <c r="D5" s="1">
         <v>45924.615481122688</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" t="s">
         <v>290</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" t="s">
         <v>291</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>26</v>
       </c>
       <c r="C6">
@@ -12163,21 +12162,21 @@
       <c r="D6" s="1">
         <v>45924.61553127315</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" t="s">
         <v>292</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" t="s">
         <v>293</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>26</v>
       </c>
       <c r="C7">
@@ -12186,21 +12185,21 @@
       <c r="D7" s="1">
         <v>45924.615590162037</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" t="s">
         <v>294</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" t="s">
         <v>295</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>26</v>
       </c>
       <c r="C8">
@@ -12209,21 +12208,21 @@
       <c r="D8" s="1">
         <v>45924.615639583331</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" t="s">
         <v>296</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" t="s">
         <v>297</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>26</v>
       </c>
       <c r="C9">
@@ -12232,21 +12231,21 @@
       <c r="D9" s="1">
         <v>45924.615694085645</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" t="s">
         <v>298</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" t="s">
         <v>299</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>26</v>
       </c>
       <c r="C10">
@@ -12255,21 +12254,21 @@
       <c r="D10" s="1">
         <v>45924.61577369213</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" t="s">
         <v>300</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" t="s">
         <v>301</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>26</v>
       </c>
       <c r="C11">
@@ -12278,21 +12277,21 @@
       <c r="D11" s="1">
         <v>45924.615872569448</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" t="s">
         <v>302</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" t="s">
         <v>303</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>26</v>
       </c>
       <c r="C12">
@@ -12301,21 +12300,21 @@
       <c r="D12" s="1">
         <v>45924.616004340278</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" t="s">
         <v>306</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" t="s">
         <v>307</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>26</v>
       </c>
       <c r="C13">
@@ -12324,21 +12323,21 @@
       <c r="D13" s="1">
         <v>45924.616055069448</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" t="s">
         <v>308</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" t="s">
         <v>309</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
       <c r="C14">
@@ -12347,21 +12346,21 @@
       <c r="D14" s="1">
         <v>45924.61610861111</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" t="s">
         <v>310</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" t="s">
         <v>311</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" t="s">
         <v>26</v>
       </c>
       <c r="C15">
@@ -12370,21 +12369,21 @@
       <c r="D15" s="1">
         <v>45924.61615858796</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" t="s">
         <v>312</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" t="s">
         <v>313</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" t="s">
         <v>26</v>
       </c>
       <c r="C16">
@@ -12393,21 +12392,21 @@
       <c r="D16" s="1">
         <v>45924.616217048613</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" t="s">
         <v>314</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" t="s">
         <v>315</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" t="s">
         <v>26</v>
       </c>
       <c r="C17">
@@ -12416,21 +12415,21 @@
       <c r="D17" s="1">
         <v>45924.616278784721</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" t="s">
         <v>316</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" t="s">
         <v>317</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" t="s">
         <v>26</v>
       </c>
       <c r="C18">
@@ -12439,21 +12438,21 @@
       <c r="D18" s="1">
         <v>45924.61633315972</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" t="s">
         <v>318</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" t="s">
         <v>319</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" t="s">
         <v>26</v>
       </c>
       <c r="C19">
@@ -12462,21 +12461,21 @@
       <c r="D19" s="1">
         <v>45924.616391053241</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" t="s">
         <v>320</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" t="s">
         <v>321</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>26</v>
       </c>
       <c r="C20">
@@ -12485,21 +12484,21 @@
       <c r="D20" s="1">
         <v>45924.616445266205</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" t="s">
         <v>322</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" t="s">
         <v>323</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" t="s">
         <v>26</v>
       </c>
       <c r="C21">
@@ -12508,21 +12507,21 @@
       <c r="D21" s="1">
         <v>45924.616500543983</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" t="s">
         <v>324</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" t="s">
         <v>325</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="C22">
@@ -12531,21 +12530,21 @@
       <c r="D22" s="1">
         <v>45924.616572708335</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" t="s">
         <v>326</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" t="s">
         <v>327</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" t="s">
         <v>135</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" t="s">
         <v>26</v>
       </c>
       <c r="C23">
@@ -12554,20 +12553,20 @@
       <c r="D23" s="1">
         <v>45924.615931828703</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" t="s">
         <v>304</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" t="s">
         <v>305</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C26">
-        <f>SUM(ex_sally_nvidia_sf100_cudf_25_10[timeMillsecs])</f>
-        <v>27129</v>
+        <f>SUM(C2:C23)</f>
+        <v>27511</v>
       </c>
     </row>
   </sheetData>
@@ -12580,10 +12579,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF739801-3399-614A-A57E-3CFACF6C119E}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12621,10 +12620,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>26</v>
       </c>
       <c r="C2">
@@ -12633,21 +12632,21 @@
       <c r="D2" s="1">
         <v>45909.61993335648</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s">
         <v>328</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" t="s">
         <v>329</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>26</v>
       </c>
       <c r="C3">
@@ -12656,21 +12655,21 @@
       <c r="D3" s="1">
         <v>45909.619993379631</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" t="s">
         <v>330</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" t="s">
         <v>331</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>26</v>
       </c>
       <c r="C4">
@@ -12679,21 +12678,21 @@
       <c r="D4" s="1">
         <v>45909.620054976855</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>332</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>333</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>26</v>
       </c>
       <c r="C5">
@@ -12702,21 +12701,21 @@
       <c r="D5" s="1">
         <v>45909.620111759257</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" t="s">
         <v>334</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" t="s">
         <v>335</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>26</v>
       </c>
       <c r="C6">
@@ -12725,21 +12724,21 @@
       <c r="D6" s="1">
         <v>45909.620163263891</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" t="s">
         <v>336</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" t="s">
         <v>337</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>26</v>
       </c>
       <c r="C7">
@@ -12748,21 +12747,21 @@
       <c r="D7" s="1">
         <v>45909.620227222222</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" t="s">
         <v>338</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" t="s">
         <v>339</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>26</v>
       </c>
       <c r="C8">
@@ -12771,21 +12770,21 @@
       <c r="D8" s="1">
         <v>45909.620276712965</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" t="s">
         <v>340</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" t="s">
         <v>341</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>26</v>
       </c>
       <c r="C9">
@@ -12794,21 +12793,21 @@
       <c r="D9" s="1">
         <v>45909.620337986111</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" t="s">
         <v>342</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" t="s">
         <v>74</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>26</v>
       </c>
       <c r="C10">
@@ -12817,21 +12816,21 @@
       <c r="D10" s="1">
         <v>45909.620431365744</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" t="s">
         <v>343</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" t="s">
         <v>344</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>26</v>
       </c>
       <c r="C11">
@@ -12840,21 +12839,21 @@
       <c r="D11" s="1">
         <v>45909.620527164348</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" t="s">
         <v>345</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" t="s">
         <v>346</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>26</v>
       </c>
       <c r="C12">
@@ -12863,21 +12862,21 @@
       <c r="D12" s="1">
         <v>45909.620638136577</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" t="s">
         <v>349</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" t="s">
         <v>350</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>26</v>
       </c>
       <c r="C13">
@@ -12886,21 +12885,21 @@
       <c r="D13" s="1">
         <v>45909.620690277778</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" t="s">
         <v>351</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" t="s">
         <v>352</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
       <c r="C14">
@@ -12909,21 +12908,21 @@
       <c r="D14" s="1">
         <v>45909.620744513886</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" t="s">
         <v>353</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" t="s">
         <v>354</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" t="s">
         <v>26</v>
       </c>
       <c r="C15">
@@ -12932,21 +12931,21 @@
       <c r="D15" s="1">
         <v>45909.620795682873</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" t="s">
         <v>355</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" t="s">
         <v>303</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" t="s">
         <v>26</v>
       </c>
       <c r="C16">
@@ -12955,21 +12954,21 @@
       <c r="D16" s="1">
         <v>45909.620855462963</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" t="s">
         <v>356</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" t="s">
         <v>357</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" t="s">
         <v>26</v>
       </c>
       <c r="C17">
@@ -12978,21 +12977,21 @@
       <c r="D17" s="1">
         <v>45909.620919224537</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" t="s">
         <v>358</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" t="s">
         <v>359</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" t="s">
         <v>26</v>
       </c>
       <c r="C18">
@@ -13001,21 +13000,21 @@
       <c r="D18" s="1">
         <v>45909.620976331018</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" t="s">
         <v>360</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" t="s">
         <v>361</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" t="s">
         <v>26</v>
       </c>
       <c r="C19">
@@ -13024,21 +13023,21 @@
       <c r="D19" s="1">
         <v>45909.621045729167</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" t="s">
         <v>362</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" t="s">
         <v>363</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>26</v>
       </c>
       <c r="C20">
@@ -13047,21 +13046,21 @@
       <c r="D20" s="1">
         <v>45909.621099027776</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" t="s">
         <v>364</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" t="s">
         <v>365</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" t="s">
         <v>26</v>
       </c>
       <c r="C21">
@@ -13070,21 +13069,21 @@
       <c r="D21" s="1">
         <v>45909.621158576389</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" t="s">
         <v>366</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" t="s">
         <v>299</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="C22">
@@ -13093,21 +13092,21 @@
       <c r="D22" s="1">
         <v>45909.621238368054</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" t="s">
         <v>367</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" t="s">
         <v>368</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" t="s">
         <v>135</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" t="s">
         <v>26</v>
       </c>
       <c r="C23">
@@ -13116,14 +13115,20 @@
       <c r="D23" s="1">
         <v>45909.620587187499</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" t="s">
         <v>347</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" t="s">
         <v>348</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>4</v>
+      <c r="G23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <f>SUM(C2:C23)</f>
+        <v>31679</v>
       </c>
     </row>
   </sheetData>

</xml_diff>